<commit_message>
site cercle: ajout du débiteur, bilan des perms
</commit_message>
<xml_diff>
--- a/site_mobilite/documents/sav_BDD/BDD_Parcours_02-10-2017_14h52.xlsx
+++ b/site_mobilite/documents/sav_BDD/BDD_Parcours_02-10-2017_14h52.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="385">
   <si>
     <t xml:space="preserve">EXP2</t>
   </si>
@@ -101,7 +101,7 @@
     <t xml:space="preserve">Maxime</t>
   </si>
   <si>
-    <t xml:space="preserve">MAT/BIO/T1</t>
+    <t xml:space="preserve">MAT/BIO</t>
   </si>
   <si>
     <t xml:space="preserve">2016-07-14</t>
@@ -1171,12 +1171,6 @@
   </si>
   <si>
     <t xml:space="preserve">DES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T1</t>
   </si>
   <si>
     <t xml:space="preserve">Management</t>
@@ -1388,24 +1382,24 @@
   </sheetPr>
   <dimension ref="A1:L93"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.89068825910931"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.9514170040486"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="119.651821862348"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.3805668016194"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="120.724696356275"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.89068825910931"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.5991902834008"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.3117408906883"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="33.4210526315789"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="26.1376518218623"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.7085020242915"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="28.7085020242915"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.919028340081"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.6356275303644"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="33.7408906882591"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.2105263157895"/>
     <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -4344,17 +4338,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.39271255060729"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.6720647773279"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="137.218623481781"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.9919028340081"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="138.506072874494"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -4634,35 +4628,20 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3" t="n">
-        <v>39</v>
-      </c>
+      <c r="A26" s="3"/>
       <c r="B26" s="3" t="s">
         <v>383</v>
       </c>
       <c r="C26" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3" t="n">
-        <v>40</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>385</v>
-      </c>
       <c r="C27" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3" t="n">
-        <v>41</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>386</v>
-      </c>
-      <c r="C28" s="3" t="s">
         <v>217</v>
       </c>
     </row>

</xml_diff>